<commit_message>
Inititalisation order fixed and norm updates
</commit_message>
<xml_diff>
--- a/Heat transition tipping pathways/_export_results.xlsx
+++ b/Heat transition tipping pathways/_export_results.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="9">
   <si>
     <t>year</t>
   </si>
@@ -370,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
@@ -407,19 +407,19 @@
         <v>2023.0</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>24334.0</v>
+        <v>214592.0</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>180.0</v>
+        <v>23037.0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>436.0</v>
+        <v>1956.0</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>984.0</v>
+        <v>11363.0</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>0.0</v>
+        <v>29829.0</v>
       </c>
     </row>
     <row r="3">
@@ -428,19 +428,19 @@
         <v>2024.0</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>24174.0</v>
+        <v>207134.0</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>165.0</v>
+        <v>19479.0</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>719.0</v>
+        <v>10002.0</v>
       </c>
       <c r="F3" s="0" t="n">
-        <v>876.0</v>
+        <v>10139.0</v>
       </c>
       <c r="G3" s="0" t="n">
-        <v>0.0</v>
+        <v>34023.0</v>
       </c>
     </row>
     <row r="4">
@@ -449,19 +449,19 @@
         <v>2025.0</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>24036.0</v>
+        <v>203183.0</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>161.0</v>
+        <v>17740.0</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>923.0</v>
+        <v>14202.0</v>
       </c>
       <c r="F4" s="0" t="n">
-        <v>814.0</v>
+        <v>9521.0</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>0.0</v>
+        <v>36131.0</v>
       </c>
     </row>
     <row r="5">
@@ -470,19 +470,19 @@
         <v>2026.0</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>23895.0</v>
+        <v>198687.0</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>159.0</v>
+        <v>15971.0</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>1144.0</v>
+        <v>19100.0</v>
       </c>
       <c r="F5" s="0" t="n">
-        <v>736.0</v>
+        <v>8896.0</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>0.0</v>
+        <v>38123.0</v>
       </c>
     </row>
     <row r="6">
@@ -491,19 +491,19 @@
         <v>2027.0</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>23769.0</v>
+        <v>193971.0</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>150.0</v>
+        <v>14209.0</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1346.0</v>
+        <v>24221.0</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>669.0</v>
+        <v>8300.0</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>0.0</v>
+        <v>40076.0</v>
       </c>
     </row>
     <row r="7">
@@ -512,19 +512,19 @@
         <v>2028.0</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>23609.0</v>
+        <v>189006.0</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>143.0</v>
+        <v>12429.0</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1566.0</v>
+        <v>29670.0</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>616.0</v>
+        <v>7712.0</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>0.0</v>
+        <v>41960.0</v>
       </c>
     </row>
     <row r="8">
@@ -535,19 +535,19 @@
         <v>2029.0</v>
       </c>
       <c r="C8" t="n" s="0">
-        <v>23435.0</v>
+        <v>183519.0</v>
       </c>
       <c r="D8" t="n" s="0">
-        <v>136.0</v>
+        <v>10710.0</v>
       </c>
       <c r="E8" t="n" s="0">
-        <v>1809.0</v>
+        <v>35398.0</v>
       </c>
       <c r="F8" t="n" s="0">
-        <v>554.0</v>
+        <v>7197.0</v>
       </c>
       <c r="G8" t="n" s="0">
-        <v>0.0</v>
+        <v>43953.0</v>
       </c>
     </row>
     <row r="9">
@@ -558,19 +558,19 @@
         <v>2030.0</v>
       </c>
       <c r="C9" t="n" s="0">
-        <v>23304.0</v>
+        <v>178004.0</v>
       </c>
       <c r="D9" t="n" s="0">
-        <v>128.0</v>
+        <v>8874.0</v>
       </c>
       <c r="E9" t="n" s="0">
-        <v>2009.0</v>
+        <v>41352.0</v>
       </c>
       <c r="F9" t="n" s="0">
-        <v>493.0</v>
+        <v>6597.0</v>
       </c>
       <c r="G9" t="n" s="0">
-        <v>0.0</v>
+        <v>45950.0</v>
       </c>
     </row>
     <row r="10">
@@ -581,19 +581,19 @@
         <v>2031.0</v>
       </c>
       <c r="C10" t="n" s="0">
-        <v>23132.0</v>
+        <v>172286.0</v>
       </c>
       <c r="D10" t="n" s="0">
-        <v>123.0</v>
+        <v>7087.0</v>
       </c>
       <c r="E10" t="n" s="0">
-        <v>2246.0</v>
+        <v>47489.0</v>
       </c>
       <c r="F10" t="n" s="0">
-        <v>433.0</v>
+        <v>6030.0</v>
       </c>
       <c r="G10" t="n" s="0">
-        <v>0.0</v>
+        <v>47885.0</v>
       </c>
     </row>
     <row r="11">
@@ -604,19 +604,19 @@
         <v>2032.0</v>
       </c>
       <c r="C11" t="n" s="0">
-        <v>22940.0</v>
+        <v>166272.0</v>
       </c>
       <c r="D11" t="n" s="0">
-        <v>119.0</v>
+        <v>5299.0</v>
       </c>
       <c r="E11" t="n" s="0">
-        <v>2509.0</v>
+        <v>53935.0</v>
       </c>
       <c r="F11" t="n" s="0">
-        <v>366.0</v>
+        <v>5502.0</v>
       </c>
       <c r="G11" t="n" s="0">
-        <v>0.0</v>
+        <v>49769.0</v>
       </c>
     </row>
     <row r="12">
@@ -627,19 +627,19 @@
         <v>2033.0</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>22758.0</v>
+        <v>159990.0</v>
       </c>
       <c r="D12" t="n" s="0">
-        <v>114.0</v>
+        <v>3539.0</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>2755.0</v>
+        <v>60644.0</v>
       </c>
       <c r="F12" t="n" s="0">
-        <v>307.0</v>
+        <v>4904.0</v>
       </c>
       <c r="G12" t="n" s="0">
-        <v>0.0</v>
+        <v>51700.0</v>
       </c>
     </row>
     <row r="13">
@@ -650,19 +650,19 @@
         <v>2034.0</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>22545.0</v>
+        <v>153524.0</v>
       </c>
       <c r="D13" t="n" s="0">
-        <v>114.0</v>
+        <v>1792.0</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>3042.0</v>
+        <v>67657.0</v>
       </c>
       <c r="F13" t="n" s="0">
-        <v>233.0</v>
+        <v>4344.0</v>
       </c>
       <c r="G13" t="n" s="0">
-        <v>0.0</v>
+        <v>53460.0</v>
       </c>
     </row>
     <row r="14">
@@ -673,19 +673,19 @@
         <v>2035.0</v>
       </c>
       <c r="C14" t="n" s="0">
-        <v>22365.0</v>
+        <v>146888.0</v>
       </c>
       <c r="D14" t="n" s="0">
-        <v>110.0</v>
+        <v>0.0</v>
       </c>
       <c r="E14" t="n" s="0">
-        <v>3298.0</v>
+        <v>74835.0</v>
       </c>
       <c r="F14" t="n" s="0">
-        <v>161.0</v>
+        <v>3751.0</v>
       </c>
       <c r="G14" t="n" s="0">
-        <v>0.0</v>
+        <v>55303.0</v>
       </c>
     </row>
     <row r="15">
@@ -696,19 +696,19 @@
         <v>2036.0</v>
       </c>
       <c r="C15" t="n" s="0">
-        <v>22175.0</v>
+        <v>141364.0</v>
       </c>
       <c r="D15" t="n" s="0">
-        <v>94.0</v>
+        <v>0.0</v>
       </c>
       <c r="E15" t="n" s="0">
-        <v>3553.0</v>
+        <v>81459.0</v>
       </c>
       <c r="F15" t="n" s="0">
-        <v>112.0</v>
+        <v>3029.0</v>
       </c>
       <c r="G15" t="n" s="0">
-        <v>0.0</v>
+        <v>54925.0</v>
       </c>
     </row>
     <row r="16">
@@ -719,19 +719,19 @@
         <v>2037.0</v>
       </c>
       <c r="C16" t="n" s="0">
-        <v>22086.0</v>
+        <v>138260.0</v>
       </c>
       <c r="D16" t="n" s="0">
-        <v>80.0</v>
+        <v>0.0</v>
       </c>
       <c r="E16" t="n" s="0">
-        <v>3712.0</v>
+        <v>85640.0</v>
       </c>
       <c r="F16" t="n" s="0">
-        <v>56.0</v>
+        <v>2326.0</v>
       </c>
       <c r="G16" t="n" s="0">
-        <v>0.0</v>
+        <v>54551.0</v>
       </c>
     </row>
     <row r="17">
@@ -742,19 +742,19 @@
         <v>2038.0</v>
       </c>
       <c r="C17" t="n" s="0">
-        <v>22000.0</v>
+        <v>135370.0</v>
       </c>
       <c r="D17" t="n" s="0">
-        <v>69.0</v>
+        <v>0.0</v>
       </c>
       <c r="E17" t="n" s="0">
-        <v>3865.0</v>
+        <v>89700.0</v>
       </c>
       <c r="F17" t="n" s="0">
-        <v>0.0</v>
+        <v>1590.0</v>
       </c>
       <c r="G17" t="n" s="0">
-        <v>0.0</v>
+        <v>54117.0</v>
       </c>
     </row>
     <row r="18">
@@ -765,19 +765,19 @@
         <v>2039.0</v>
       </c>
       <c r="C18" t="n" s="0">
-        <v>21851.0</v>
+        <v>136929.0</v>
       </c>
       <c r="D18" t="n" s="0">
-        <v>65.0</v>
+        <v>0.0</v>
       </c>
       <c r="E18" t="n" s="0">
-        <v>4018.0</v>
+        <v>88802.0</v>
       </c>
       <c r="F18" t="n" s="0">
-        <v>0.0</v>
+        <v>1398.0</v>
       </c>
       <c r="G18" t="n" s="0">
-        <v>0.0</v>
+        <v>53648.0</v>
       </c>
     </row>
     <row r="19">
@@ -788,19 +788,19 @@
         <v>2040.0</v>
       </c>
       <c r="C19" t="n" s="0">
-        <v>21657.0</v>
+        <v>134788.0</v>
       </c>
       <c r="D19" t="n" s="0">
-        <v>56.0</v>
+        <v>0.0</v>
       </c>
       <c r="E19" t="n" s="0">
-        <v>4221.0</v>
+        <v>91585.0</v>
       </c>
       <c r="F19" t="n" s="0">
-        <v>0.0</v>
+        <v>1306.0</v>
       </c>
       <c r="G19" t="n" s="0">
-        <v>0.0</v>
+        <v>53098.0</v>
       </c>
     </row>
     <row r="20">
@@ -811,19 +811,19 @@
         <v>2041.0</v>
       </c>
       <c r="C20" t="n" s="0">
-        <v>21465.0</v>
+        <v>132010.0</v>
       </c>
       <c r="D20" t="n" s="0">
-        <v>47.0</v>
+        <v>0.0</v>
       </c>
       <c r="E20" t="n" s="0">
-        <v>4422.0</v>
+        <v>94921.0</v>
       </c>
       <c r="F20" t="n" s="0">
-        <v>0.0</v>
+        <v>1224.0</v>
       </c>
       <c r="G20" t="n" s="0">
-        <v>0.0</v>
+        <v>52622.0</v>
       </c>
     </row>
     <row r="21">
@@ -834,19 +834,19 @@
         <v>2042.0</v>
       </c>
       <c r="C21" t="n" s="0">
-        <v>21271.0</v>
+        <v>128991.0</v>
       </c>
       <c r="D21" t="n" s="0">
-        <v>43.0</v>
+        <v>0.0</v>
       </c>
       <c r="E21" t="n" s="0">
-        <v>4620.0</v>
+        <v>98496.0</v>
       </c>
       <c r="F21" t="n" s="0">
-        <v>0.0</v>
+        <v>1137.0</v>
       </c>
       <c r="G21" t="n" s="0">
-        <v>0.0</v>
+        <v>52153.0</v>
       </c>
     </row>
     <row r="22">
@@ -857,19 +857,19 @@
         <v>2043.0</v>
       </c>
       <c r="C22" t="n" s="0">
-        <v>21025.0</v>
+        <v>125805.0</v>
       </c>
       <c r="D22" t="n" s="0">
-        <v>33.0</v>
+        <v>0.0</v>
       </c>
       <c r="E22" t="n" s="0">
-        <v>4876.0</v>
+        <v>102251.0</v>
       </c>
       <c r="F22" t="n" s="0">
-        <v>0.0</v>
+        <v>1040.0</v>
       </c>
       <c r="G22" t="n" s="0">
-        <v>0.0</v>
+        <v>51681.0</v>
       </c>
     </row>
     <row r="23">
@@ -880,19 +880,19 @@
         <v>2044.0</v>
       </c>
       <c r="C23" t="n" s="0">
-        <v>20774.0</v>
+        <v>122405.0</v>
       </c>
       <c r="D23" t="n" s="0">
-        <v>33.0</v>
+        <v>0.0</v>
       </c>
       <c r="E23" t="n" s="0">
-        <v>5127.0</v>
+        <v>106258.0</v>
       </c>
       <c r="F23" t="n" s="0">
-        <v>0.0</v>
+        <v>939.0</v>
       </c>
       <c r="G23" t="n" s="0">
-        <v>0.0</v>
+        <v>51175.0</v>
       </c>
     </row>
     <row r="24">
@@ -903,19 +903,19 @@
         <v>2045.0</v>
       </c>
       <c r="C24" t="n" s="0">
-        <v>20495.0</v>
+        <v>118944.0</v>
       </c>
       <c r="D24" t="n" s="0">
-        <v>33.0</v>
+        <v>0.0</v>
       </c>
       <c r="E24" t="n" s="0">
-        <v>5406.0</v>
+        <v>110286.0</v>
       </c>
       <c r="F24" t="n" s="0">
-        <v>0.0</v>
+        <v>863.0</v>
       </c>
       <c r="G24" t="n" s="0">
-        <v>0.0</v>
+        <v>50684.0</v>
       </c>
     </row>
     <row r="25">
@@ -926,19 +926,19 @@
         <v>2046.0</v>
       </c>
       <c r="C25" t="n" s="0">
-        <v>20209.0</v>
+        <v>115423.0</v>
       </c>
       <c r="D25" t="n" s="0">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
       <c r="E25" t="n" s="0">
-        <v>5693.0</v>
+        <v>114314.0</v>
       </c>
       <c r="F25" t="n" s="0">
-        <v>0.0</v>
+        <v>778.0</v>
       </c>
       <c r="G25" t="n" s="0">
-        <v>0.0</v>
+        <v>50262.0</v>
       </c>
     </row>
     <row r="26">
@@ -949,19 +949,19 @@
         <v>2047.0</v>
       </c>
       <c r="C26" t="n" s="0">
-        <v>19898.0</v>
+        <v>111961.0</v>
       </c>
       <c r="D26" t="n" s="0">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
       <c r="E26" t="n" s="0">
-        <v>6004.0</v>
+        <v>118311.0</v>
       </c>
       <c r="F26" t="n" s="0">
-        <v>0.0</v>
+        <v>676.0</v>
       </c>
       <c r="G26" t="n" s="0">
-        <v>0.0</v>
+        <v>49829.0</v>
       </c>
     </row>
     <row r="27">
@@ -972,19 +972,19 @@
         <v>2048.0</v>
       </c>
       <c r="C27" t="n" s="0">
-        <v>19241.0</v>
+        <v>103623.0</v>
       </c>
       <c r="D27" t="n" s="0">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
       <c r="E27" t="n" s="0">
-        <v>6661.0</v>
+        <v>127060.0</v>
       </c>
       <c r="F27" t="n" s="0">
-        <v>0.0</v>
+        <v>603.0</v>
       </c>
       <c r="G27" t="n" s="0">
-        <v>0.0</v>
+        <v>49491.0</v>
       </c>
     </row>
     <row r="28">
@@ -995,19 +995,19 @@
         <v>2049.0</v>
       </c>
       <c r="C28" t="n" s="0">
-        <v>18932.0</v>
+        <v>99939.0</v>
       </c>
       <c r="D28" t="n" s="0">
-        <v>32.0</v>
+        <v>0.0</v>
       </c>
       <c r="E28" t="n" s="0">
-        <v>6970.0</v>
+        <v>131353.0</v>
       </c>
       <c r="F28" t="n" s="0">
-        <v>0.0</v>
+        <v>513.0</v>
       </c>
       <c r="G28" t="n" s="0">
-        <v>0.0</v>
+        <v>48972.0</v>
       </c>
     </row>
     <row r="29">
@@ -1018,19 +1018,19 @@
         <v>2050.0</v>
       </c>
       <c r="C29" t="n" s="0">
-        <v>18630.0</v>
+        <v>96553.0</v>
       </c>
       <c r="D29" t="n" s="0">
-        <v>31.0</v>
+        <v>0.0</v>
       </c>
       <c r="E29" t="n" s="0">
-        <v>7273.0</v>
+        <v>135311.0</v>
       </c>
       <c r="F29" t="n" s="0">
-        <v>0.0</v>
+        <v>418.0</v>
       </c>
       <c r="G29" t="n" s="0">
-        <v>0.0</v>
+        <v>48495.0</v>
       </c>
     </row>
     <row r="30">
@@ -1038,19 +1038,22 @@
         <v>2051.0</v>
       </c>
       <c r="B30" t="n" s="0">
-        <v>195436.0</v>
+        <v>2066.0</v>
       </c>
       <c r="C30" t="n" s="0">
-        <v>4284.0</v>
+        <v>53769.0</v>
       </c>
       <c r="D30" t="n" s="0">
-        <v>72059.0</v>
+        <v>0.0</v>
       </c>
       <c r="E30" t="n" s="0">
-        <v>5.0</v>
+        <v>170079.0</v>
       </c>
       <c r="F30" t="n" s="0">
-        <v>8993.0</v>
+        <v>7415.0</v>
+      </c>
+      <c r="G30" t="n" s="0">
+        <v>49514.0</v>
       </c>
     </row>
     <row r="31">
@@ -1058,19 +1061,22 @@
         <v>2052.0</v>
       </c>
       <c r="B31" t="n" s="0">
-        <v>193425.0</v>
+        <v>2067.0</v>
       </c>
       <c r="C31" t="n" s="0">
-        <v>4276.0</v>
+        <v>52816.0</v>
       </c>
       <c r="D31" t="n" s="0">
-        <v>74956.0</v>
+        <v>0.0</v>
       </c>
       <c r="E31" t="n" s="0">
-        <v>5.0</v>
+        <v>171242.0</v>
       </c>
       <c r="F31" t="n" s="0">
-        <v>8115.0</v>
+        <v>7413.0</v>
+      </c>
+      <c r="G31" t="n" s="0">
+        <v>49306.0</v>
       </c>
     </row>
     <row r="32">
@@ -1078,19 +1084,202 @@
         <v>2053.0</v>
       </c>
       <c r="B32" t="n" s="0">
-        <v>191338.0</v>
+        <v>2068.0</v>
       </c>
       <c r="C32" t="n" s="0">
-        <v>4281.0</v>
+        <v>51886.0</v>
       </c>
       <c r="D32" t="n" s="0">
-        <v>77930.0</v>
+        <v>0.0</v>
       </c>
       <c r="E32" t="n" s="0">
-        <v>5.0</v>
+        <v>172402.0</v>
       </c>
       <c r="F32" t="n" s="0">
-        <v>7223.0</v>
+        <v>7413.0</v>
+      </c>
+      <c r="G32" t="n" s="0">
+        <v>49076.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="n" s="0">
+        <v>2069.0</v>
+      </c>
+      <c r="C33" t="n" s="0">
+        <v>51044.0</v>
+      </c>
+      <c r="D33" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E33" t="n" s="0">
+        <v>173462.0</v>
+      </c>
+      <c r="F33" t="n" s="0">
+        <v>7389.0</v>
+      </c>
+      <c r="G33" t="n" s="0">
+        <v>48882.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="n" s="0">
+        <v>2070.0</v>
+      </c>
+      <c r="C34" t="n" s="0">
+        <v>50250.0</v>
+      </c>
+      <c r="D34" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E34" t="n" s="0">
+        <v>174459.0</v>
+      </c>
+      <c r="F34" t="n" s="0">
+        <v>7391.0</v>
+      </c>
+      <c r="G34" t="n" s="0">
+        <v>48677.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="n" s="0">
+        <v>2071.0</v>
+      </c>
+      <c r="C35" t="n" s="0">
+        <v>49428.0</v>
+      </c>
+      <c r="D35" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E35" t="n" s="0">
+        <v>175512.0</v>
+      </c>
+      <c r="F35" t="n" s="0">
+        <v>7384.0</v>
+      </c>
+      <c r="G35" t="n" s="0">
+        <v>48453.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="n" s="0">
+        <v>2072.0</v>
+      </c>
+      <c r="C36" t="n" s="0">
+        <v>48024.0</v>
+      </c>
+      <c r="D36" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E36" t="n" s="0">
+        <v>177088.0</v>
+      </c>
+      <c r="F36" t="n" s="0">
+        <v>7350.0</v>
+      </c>
+      <c r="G36" t="n" s="0">
+        <v>48315.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="n" s="0">
+        <v>2073.0</v>
+      </c>
+      <c r="C37" t="n" s="0">
+        <v>47326.0</v>
+      </c>
+      <c r="D37" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E37" t="n" s="0">
+        <v>177994.0</v>
+      </c>
+      <c r="F37" t="n" s="0">
+        <v>7309.0</v>
+      </c>
+      <c r="G37" t="n" s="0">
+        <v>48148.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="n" s="0">
+        <v>2074.0</v>
+      </c>
+      <c r="C38" t="n" s="0">
+        <v>46685.0</v>
+      </c>
+      <c r="D38" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E38" t="n" s="0">
+        <v>178858.0</v>
+      </c>
+      <c r="F38" t="n" s="0">
+        <v>7265.0</v>
+      </c>
+      <c r="G38" t="n" s="0">
+        <v>47969.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="n" s="0">
+        <v>2075.0</v>
+      </c>
+      <c r="C39" t="n" s="0">
+        <v>46068.0</v>
+      </c>
+      <c r="D39" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E39" t="n" s="0">
+        <v>179684.0</v>
+      </c>
+      <c r="F39" t="n" s="0">
+        <v>7222.0</v>
+      </c>
+      <c r="G39" t="n" s="0">
+        <v>47803.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="n" s="0">
+        <v>2076.0</v>
+      </c>
+      <c r="C40" t="n" s="0">
+        <v>45498.0</v>
+      </c>
+      <c r="D40" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E40" t="n" s="0">
+        <v>180470.0</v>
+      </c>
+      <c r="F40" t="n" s="0">
+        <v>7191.0</v>
+      </c>
+      <c r="G40" t="n" s="0">
+        <v>47618.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="n" s="0">
+        <v>2077.0</v>
+      </c>
+      <c r="C41" t="n" s="0">
+        <v>44959.0</v>
+      </c>
+      <c r="D41" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E41" t="n" s="0">
+        <v>181232.0</v>
+      </c>
+      <c r="F41" t="n" s="0">
+        <v>7154.0</v>
+      </c>
+      <c r="G41" t="n" s="0">
+        <v>47432.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>